<commit_message>
arreglando unas fechas que estaban mal escritas
</commit_message>
<xml_diff>
--- a/topeducation/examen.xlsx
+++ b/topeducation/examen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\2-2023\MINGESO\proyecto-mingeso\topeducation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0A767DD-D764-4FCB-8312-5B4ED0C2FB1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7AD7C5-FDD3-41AB-AEC5-3B82292C7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6458D67F-A596-4B9E-98DC-F62F15BBE9B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>rut</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>20.285.942-3</t>
+  </si>
+  <si>
+    <t>123.123.123</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574F55A7-86D2-494C-BBA7-13891E765C20}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="A1:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,6 +518,17 @@
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C9" s="2">
+        <v>900</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
test antes de la prueba
</commit_message>
<xml_diff>
--- a/topeducation/examen.xlsx
+++ b/topeducation/examen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\2-2023\MINGESO\proyecto-mingeso\topeducation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF7AD7C5-FDD3-41AB-AEC5-3B82292C7BD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD8D47-5815-46D8-874E-18FEDDB0D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6458D67F-A596-4B9E-98DC-F62F15BBE9B5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>rut</t>
   </si>
@@ -68,15 +68,26 @@
     <t>20.285.942-3</t>
   </si>
   <si>
-    <t>123.123.123</t>
+    <t>rut1</t>
+  </si>
+  <si>
+    <t>rut2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -104,10 +115,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -422,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574F55A7-86D2-494C-BBA7-13891E765C20}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="A1:C9"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +541,20 @@
         <v>900</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1">
+        <v>45198</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
microservicio 2 listo con las 3 funcionalidades expuestas en la api, además se refactorizo código con mejores prácticas (uso de DTOS), por otro lado, se estructura el microservicio 3 y se completa la funcionalidad para importar exámenes en él.
</commit_message>
<xml_diff>
--- a/topeducation/examen.xlsx
+++ b/topeducation/examen.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hector\Documents\2-2023\MINGESO\proyecto-mingeso\topeducation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyecto-mingeso\topeducation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2CD8D47-5815-46D8-874E-18FEDDB0D5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59BD2D51-30BD-49CB-9A7D-89098477BA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{6458D67F-A596-4B9E-98DC-F62F15BBE9B5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>rut</t>
   </si>
@@ -47,47 +47,18 @@
     <t>puntaje</t>
   </si>
   <si>
-    <t>19.234.554-8</t>
-  </si>
-  <si>
-    <t>20.234.343-7</t>
-  </si>
-  <si>
-    <t>18.544.321-5</t>
-  </si>
-  <si>
-    <t>12.345.234-2</t>
-  </si>
-  <si>
-    <t>19.234.235-8</t>
-  </si>
-  <si>
-    <t>12.345.234-1</t>
-  </si>
-  <si>
-    <t>20.285.942-3</t>
-  </si>
-  <si>
     <t>rut1</t>
   </si>
   <si>
-    <t>rut2</t>
+    <t>20.999.124-8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -115,11 +86,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,127 +405,50 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{574F55A7-86D2-494C-BBA7-13891E765C20}">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3FBC4E4-2915-4092-A97C-01204A5B7027}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
+      <c r="A2" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="1">
-        <v>45198</v>
+        <v>45226</v>
       </c>
       <c r="C2" s="2">
-        <v>900</v>
+        <v>950</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>45198</v>
+        <v>45226</v>
       </c>
       <c r="C3" s="2">
-        <v>860</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C4" s="2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C5" s="2">
-        <v>800</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C6" s="2">
-        <v>988</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C7" s="2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C9" s="2">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>45198</v>
-      </c>
-      <c r="C10" s="2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+        <v>980</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>